<commit_message>
prove null hypothesis to be rejected using t ttest_ind
</commit_message>
<xml_diff>
--- a/Results-Generation/subj1/results_Alpha.xlsx
+++ b/Results-Generation/subj1/results_Alpha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Layers Number</t>
   </si>
@@ -79,19 +79,10 @@
     <t>Noise</t>
   </si>
   <si>
-    <t>eyescrunching</t>
-  </si>
-  <si>
-    <t>jaw</t>
-  </si>
-  <si>
-    <t>raisingeyebrows</t>
-  </si>
-  <si>
-    <t>movehat</t>
-  </si>
-  <si>
-    <t>movehead</t>
+    <t>eyescrunching+jaw</t>
+  </si>
+  <si>
+    <t>jaw+raisingeyebrows</t>
   </si>
 </sst>
 </file>
@@ -449,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,13 +561,13 @@
         <v>0.01</v>
       </c>
       <c r="Q2">
-        <v>-0.1006357881055001</v>
+        <v>-1.712258434503343</v>
       </c>
       <c r="R2">
-        <v>18.88297917915416</v>
+        <v>4.320651653371465</v>
       </c>
       <c r="S2">
-        <v>10.33780268370426</v>
+        <v>-2.967762154706217</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -635,214 +626,19 @@
         <v>0.1</v>
       </c>
       <c r="Q3">
-        <v>-0.9857359524090255</v>
+        <v>-1.022131778245286</v>
       </c>
       <c r="R3">
-        <v>3.093209696893958</v>
+        <v>6.42221850955547</v>
       </c>
       <c r="S3">
-        <v>-17.92678862848308</v>
+        <v>-18.82147087323878</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="U3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>2.5</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>15</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0.01</v>
-      </c>
-      <c r="P4">
-        <v>0.01</v>
-      </c>
-      <c r="Q4">
-        <v>-0.00835458213298745</v>
-      </c>
-      <c r="R4">
-        <v>28.12336853816186</v>
-      </c>
-      <c r="S4">
-        <v>23.52076023292342</v>
-      </c>
-      <c r="T4">
-        <v>2</v>
-      </c>
-      <c r="U4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2.5</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0.5</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>15</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0.01</v>
-      </c>
-      <c r="P5">
-        <v>0.01</v>
-      </c>
-      <c r="Q5">
-        <v>-0.1397546285295138</v>
-      </c>
-      <c r="R5">
-        <v>16.50099053386411</v>
-      </c>
-      <c r="S5">
-        <v>3.264118575062555</v>
-      </c>
-      <c r="T5">
-        <v>3</v>
-      </c>
-      <c r="U5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2.5</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0.5</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>15</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0.01</v>
-      </c>
-      <c r="P6">
-        <v>0.01</v>
-      </c>
-      <c r="Q6">
-        <v>-0.1463518496510229</v>
-      </c>
-      <c r="R6">
-        <v>17.57766371517265</v>
-      </c>
-      <c r="S6">
-        <v>10.7867512419778</v>
-      </c>
-      <c r="T6">
-        <v>4</v>
-      </c>
-      <c r="U6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>